<commit_message>
add data for phase and static
</commit_message>
<xml_diff>
--- a/data/conslay/phaseBuilding.xlsx
+++ b/data/conslay/phaseBuilding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daovudat/Desktop/Projects/freelance/golang-moaha-construction/data/conslay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC9677E-40AF-7D42-8033-2847D4FA1E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FAF6AD-901F-F146-9966-7AEC18BB1993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{82FBD6D4-541B-A340-931E-720121D87B31}"/>
   </bookViews>
@@ -35,36 +35,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">Interval time 1: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interval time 2: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interval time 3: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interval time 4: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interval time 5: </t>
-  </si>
-  <si>
-    <t>TF1, TF2, TF3, TF6, TF13, TF16</t>
-  </si>
-  <si>
-    <t>TF3, TF4, TF5, TF6, TF7, TF13, TF16</t>
-  </si>
-  <si>
-    <t>TF3, TF4, TF5, TF6, TF7, TF11, TF13, TF14, TF15, TF16</t>
-  </si>
-  <si>
-    <t>TF3, TF6, TF8, TF9, TF11, TF13, TF14, TF15, TF16</t>
-  </si>
-  <si>
-    <t>TF3, TF6, TF10, TF11, TF12, TF13, TF14, TF15, TF16</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">Phase 1: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phase 2: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phase 3: </t>
+  </si>
+  <si>
+    <t>TF13, TF16, TF1, TF2, TF3, TF4, TF5, TF6, TF7</t>
+  </si>
+  <si>
+    <t>TF13, TF16, TF3, TF4, TF5, TF6, TF7, TF8, TF9, TF11, TF14, TF15</t>
+  </si>
+  <si>
+    <t>TF13, TF16, TF3, TF6, TF10, TF11, TF12, TF14, TF15</t>
   </si>
 </sst>
 </file>
@@ -422,15 +410,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA024008-5D72-9649-81A4-DE7FF0B70DB1}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -438,7 +427,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -446,7 +435,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -454,23 +443,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>